<commit_message>
[INS] Graficos de disposição de memória
</commit_message>
<xml_diff>
--- a/Graficos.xlsx
+++ b/Graficos.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Workload0</t>
   </si>
@@ -76,6 +76,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEF6767"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -126,7 +131,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="pt-BR" sz="1600" b="1" baseline="0"/>
-              <a:t> bem e mal sucedidas</a:t>
+              <a:t> bem e mal sucedidas (sem aglutinação)</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR" sz="1600" b="1"/>
           </a:p>
@@ -184,9 +189,67 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$6:$C$6</c:f>
+              <c:f>worksheet!$A$6:$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -203,7 +266,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$C$4</c:f>
+              <c:f>worksheet!$A$4:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -233,7 +296,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="EF6767"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -241,9 +304,67 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$6:$C$6</c:f>
+              <c:f>worksheet!$A$6:$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -260,7 +381,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$C$5</c:f>
+              <c:f>worksheet!$A$5:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -283,8 +404,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -514,7 +636,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -648,7 +770,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="pt-BR" sz="1600" b="1" baseline="0"/>
-              <a:t> bem e mal sucedidas</a:t>
+              <a:t> bem e mal sucedidas (com aglutinação)</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR" sz="1600" b="1"/>
           </a:p>
@@ -706,9 +828,67 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$6:$C$6</c:f>
+              <c:f>worksheet!$A$6:$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -725,7 +905,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$C$7</c:f>
+              <c:f>worksheet!$A$7:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -755,7 +935,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="EF6767"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -763,9 +943,67 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$6:$C$6</c:f>
+              <c:f>worksheet!$A$6:$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -782,7 +1020,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$8:$C$8</c:f>
+              <c:f>worksheet!$A$8:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -805,8 +1043,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1038,7 +1277,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1057,6 +1296,1171 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="1"/>
+              <a:t>Espaço</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="1" baseline="0"/>
+              <a:t> Livre e nº de Regiões Difusas (com algutinação)</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1600" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Espaço Livre Total</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>worksheet!$A$11:$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Workload0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Workload1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Workload2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>worksheet!$A$12:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2029964</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2312781</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1522676</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7236-4A42-ABF8-0427C9A201A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Nº de Regiões Difusas</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>worksheet!$A$11:$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Workload0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Workload1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Workload2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>worksheet!$A$13:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7236-4A42-ABF8-0427C9A201A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="299841007"/>
+        <c:axId val="298688271"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="299841007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1200"/>
+                  <a:t>Workloads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.50520060408191769"/>
+              <c:y val="0.91717069892473102"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="298688271"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="298688271"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="4194303.9999999991"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1200"/>
+                  <a:t>Valores</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1200" baseline="0"/>
+                  <a:t> em escala log10</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.4781966001478197E-2"/>
+              <c:y val="0.31665846456692914"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299841007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="1"/>
+              <a:t>Espaço</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600" b="1" baseline="0"/>
+              <a:t> Livre e nº de Regiões Difusas (sem aglutinação)</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1600" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Espaço Livre Total</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>worksheet!$A$11:$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Workload0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Workload1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Workload2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>worksheet!$A$15:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6379537</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7647982</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9459108</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-46ED-4AF9-BF28-E29775413CB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Nº de Regiões Difusas</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>worksheet!$A$11:$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Workload0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Workload1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Workload2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>worksheet!$A$16:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4773</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4864</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4865</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-46ED-4AF9-BF28-E29775413CB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="299841007"/>
+        <c:axId val="298688271"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="299841007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1200"/>
+                  <a:t>Workloads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.50520060408191769"/>
+              <c:y val="0.91717069892473102"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="298688271"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="298688271"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1200"/>
+                  <a:t>Valores</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" sz="1200" baseline="0"/>
+                  <a:t> em escala log10</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.4781966001478197E-2"/>
+              <c:y val="0.31665846456692914"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299841007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1213,6 +2617,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -2204,6 +3688,1038 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2294,6 +4810,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{726760D4-E816-4DAA-B47D-C35916624700}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31399059-19FF-4A12-B3D7-97F13CA618C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2599,10 +5189,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="AD12" sqref="AD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2679,6 +5269,61 @@
         <v>4</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2029964</v>
+      </c>
+      <c r="B12">
+        <v>2312781</v>
+      </c>
+      <c r="C12">
+        <v>1522676</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>88</v>
+      </c>
+      <c r="B13">
+        <v>77</v>
+      </c>
+      <c r="C13">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>6379537</v>
+      </c>
+      <c r="B15">
+        <v>7647982</v>
+      </c>
+      <c r="C15">
+        <v>9459108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>4773</v>
+      </c>
+      <c r="B16">
+        <v>4864</v>
+      </c>
+      <c r="C16">
+        <v>4865</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>